<commit_message>
Add caching for data loadinggit add . Complete load_scales docu
</commit_message>
<xml_diff>
--- a/docs/source/index/tables/t0_mapper.xlsx
+++ b/docs/source/index/tables/t0_mapper.xlsx
@@ -182,10 +182,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>

</xml_diff>